<commit_message>
Second Menu Definition File Upload
</commit_message>
<xml_diff>
--- a/메뉴 정의표.xlsx
+++ b/메뉴 정의표.xlsx
@@ -1,31 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hi\Desktop\개발 자료 모음\개인 프로젝트_협업\참고자료\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E59926FF-168B-472C-857E-2D856EF27784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10E29837-EA3F-4A17-8364-FFA3F3F27B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{12DDF597-18D5-4791-8DDF-2ED924DD9A72}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{12DDF597-18D5-4791-8DDF-2ED924DD9A72}"/>
   </bookViews>
   <sheets>
-    <sheet name="메뉴 분담" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="메뉴 분담" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="45">
   <si>
     <t>No</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -159,6 +168,50 @@
   </si>
   <si>
     <t>페이지 수</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>예상 시간(주 단위)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>실제 소요시간</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공통</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>header</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>footer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>영화 영상 / 사진</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>event 밑 탭 &gt; 영화 목록 / 공지사항</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>최신영화 이미지(메인 이미지) &gt; 자동이동 / 선택이동</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>우측 따라다니는 배너 &gt; 따라다니는 기능</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>.property &gt; 약관 text를 넣고 이거를 불러오기</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>격주로 스터디룸에서 미팅</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -197,7 +250,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -220,13 +273,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -238,6 +300,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -552,25 +620,70 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C6C2CD-9435-4BC5-B544-7FB49CF310EA}">
+  <dimension ref="B3:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="1">
+        <f>SUM('메뉴 분담'!G4:G10,'메뉴 분담'!G18:G26)</f>
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.4">
+      <c r="B5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="1">
+        <f>SUM('메뉴 분담'!G11:G17,'메뉴 분담'!G27:G28)</f>
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{430EAB5E-D205-4A13-97F7-8D84586C15BB}">
-  <dimension ref="B1:J26"/>
+  <dimension ref="B1:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="4" max="4" width="10.3984375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.69921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="1" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="2:10" x14ac:dyDescent="0.4">
+    <row r="3" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -589,8 +702,17 @@
       <c r="G3" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="4" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K3" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="4" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B4" s="1">
         <v>1</v>
       </c>
@@ -605,14 +727,12 @@
       <c r="G4" s="1">
         <v>1</v>
       </c>
-      <c r="I4" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H4" s="1">
+        <v>5</v>
+      </c>
+      <c r="I4" s="1"/>
+    </row>
+    <row r="5" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B5" s="1">
         <v>2</v>
       </c>
@@ -629,15 +749,12 @@
       <c r="G5" s="1">
         <v>1</v>
       </c>
-      <c r="I5" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" s="1">
-        <f>SUM(G4:G10,G18:G26)</f>
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H5" s="1">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1"/>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B6" s="1">
         <v>3</v>
       </c>
@@ -652,15 +769,12 @@
       <c r="G6" s="1">
         <v>1</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J6" s="1">
-        <f>SUM(G11:G17)</f>
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H6" s="1">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1"/>
+    </row>
+    <row r="7" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B7" s="1">
         <v>4</v>
       </c>
@@ -677,8 +791,12 @@
       <c r="G7" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H7" s="1">
+        <v>5</v>
+      </c>
+      <c r="I7" s="1"/>
+    </row>
+    <row r="8" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B8" s="1">
         <v>5</v>
       </c>
@@ -693,8 +811,12 @@
       <c r="G8" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H8" s="1">
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B9" s="1">
         <v>6</v>
       </c>
@@ -709,8 +831,12 @@
       <c r="G9" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H9" s="1">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B10" s="1">
         <v>7</v>
       </c>
@@ -725,8 +851,12 @@
       <c r="G10" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H10" s="1">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1"/>
+    </row>
+    <row r="11" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B11" s="1">
         <v>8</v>
       </c>
@@ -741,8 +871,12 @@
       <c r="G11" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H11" s="1">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1"/>
+    </row>
+    <row r="12" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B12" s="1">
         <v>9</v>
       </c>
@@ -757,8 +891,12 @@
       <c r="G12" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H12" s="1">
+        <v>6</v>
+      </c>
+      <c r="I12" s="1"/>
+    </row>
+    <row r="13" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B13" s="1">
         <v>10</v>
       </c>
@@ -773,8 +911,12 @@
       <c r="G13" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H13" s="1">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1"/>
+    </row>
+    <row r="14" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B14" s="1">
         <v>11</v>
       </c>
@@ -789,8 +931,12 @@
       <c r="G14" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H14" s="1">
+        <v>3</v>
+      </c>
+      <c r="I14" s="1"/>
+    </row>
+    <row r="15" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B15" s="1">
         <v>12</v>
       </c>
@@ -807,8 +953,12 @@
       <c r="G15" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="H15" s="1">
+        <v>10</v>
+      </c>
+      <c r="I15" s="1"/>
+    </row>
+    <row r="16" spans="2:11" x14ac:dyDescent="0.4">
       <c r="B16" s="1">
         <v>13</v>
       </c>
@@ -823,8 +973,12 @@
       <c r="G16" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="H16" s="1">
+        <v>5</v>
+      </c>
+      <c r="I16" s="1"/>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B17" s="1">
         <v>14</v>
       </c>
@@ -839,8 +993,12 @@
       <c r="G17" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="H17" s="1">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B18" s="1">
         <v>15</v>
       </c>
@@ -855,8 +1013,12 @@
       <c r="G18" s="1">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="H18" s="1">
+        <v>0</v>
+      </c>
+      <c r="I18" s="1"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B19" s="1">
         <v>16</v>
       </c>
@@ -871,8 +1033,12 @@
       <c r="G19" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="H19" s="1">
+        <v>5</v>
+      </c>
+      <c r="I19" s="1"/>
+    </row>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B20" s="1">
         <v>17</v>
       </c>
@@ -887,8 +1053,12 @@
       <c r="G20" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="H20" s="1">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1"/>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B21" s="1">
         <v>18</v>
       </c>
@@ -903,8 +1073,12 @@
       <c r="G21" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="H21" s="1">
+        <v>3</v>
+      </c>
+      <c r="I21" s="1"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B22" s="1">
         <v>19</v>
       </c>
@@ -919,8 +1093,12 @@
       <c r="G22" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="H22" s="1">
+        <v>3</v>
+      </c>
+      <c r="I22" s="1"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B23" s="1">
         <v>20</v>
       </c>
@@ -935,8 +1113,12 @@
       <c r="G23" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="H23" s="1">
+        <v>5</v>
+      </c>
+      <c r="I23" s="1"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B24" s="1">
         <v>21</v>
       </c>
@@ -951,8 +1133,12 @@
       <c r="G24" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="H24" s="1">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B25" s="1">
         <v>22</v>
       </c>
@@ -967,8 +1153,12 @@
       <c r="G25" s="1">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="H25" s="1">
+        <v>3</v>
+      </c>
+      <c r="I25" s="1"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.4">
       <c r="B26" s="1">
         <v>23</v>
       </c>
@@ -982,6 +1172,98 @@
       </c>
       <c r="G26" s="1">
         <v>1</v>
+      </c>
+      <c r="H26" s="1">
+        <v>5</v>
+      </c>
+      <c r="I26" s="1"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B27" s="4">
+        <v>24</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G27" s="1">
+        <v>1</v>
+      </c>
+      <c r="H27" s="1">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.4">
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G28" s="1">
+        <v>1</v>
+      </c>
+      <c r="H28" s="1">
+        <v>1</v>
+      </c>
+      <c r="I28" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05590104-8478-4370-894C-DD352DD0FB22}">
+  <dimension ref="C3:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
+  <sheetData>
+    <row r="3" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="D4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="D6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="3:4" x14ac:dyDescent="0.4">
+      <c r="C9" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>